<commit_message>
Get daily reddit data: Tue Nov 26 08:11:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_01.xlsx
+++ b/data/collected_data/2024_12_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C492"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3253 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1h04s5m</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>(24f) Getting my nails done for the first time ever and I need help w/ ideas, please!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h04s5m/24f_getting_my_nails_done_for_the_first_time_ever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1h06100</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Tinsel Tones</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h06100</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1h05yyz</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>my first acrylic set i’ve done since last year ☺️</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h05yyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1h05sap</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>perfect for fall 🍁</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kptbcfki073e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1h05pfc</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s a trip to Germany without some nice nails? </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me79nmnhz63e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1h05ltj</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Un-even nail ridges?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h05ltj</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1h05j2v</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Back in the game 💜</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uyt7g07ex63e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1h054pa</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>christmassss nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ooprarts63e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1h04xq6</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>favorite matte polish</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nfuk7ifqq63e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1h04fc0</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>French-ish - neutral or pink next time?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h04fc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1h03sco</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Nail damage</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5uv3hzme63e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1h03fzi</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Anyone know a nailpolish that is close to this?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h03fzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1h02og2</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>19 in 2 days🥳💜first time with nails like these🌈💕did them myself💛</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hzfqbkxu363e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1h03azs</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is $70 a lot for a Gel Full Set?? </t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h03azs/is_70_a_lot_for_a_gel_full_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1h038j9</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>My 2024 nails album</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h038j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1h02i93</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Third time trying builder gel</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szx20zz7263e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1h0267s</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>‘tis the early season</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0267s</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1h01acq</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very demure, very mindful </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h01acq</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1h0197a</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Husband nail date 😬💅</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3s3p8f0rq53e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1h01743</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Tried tortoise shell nails!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwmg2jv7q53e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1h010c1</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>How to take better pictures with iPhone?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h010c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1h00urb</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Dipped in chocolate 🍫</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqlok5i8n53e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1h00c14</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>How bad is it? Feel like the nail tech did me dirty</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h00c14</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1gzzyhr</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>I chose the green set</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzzyhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1gzzbn7</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Is this legit?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzzbn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1gzys0i</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>My 1st try at painting my own nails!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzys0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1gzyj8l</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5o80azh353e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1gzya71</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hybrid gel extensions with Lights Lacquer polish in the shade High Fae! and yes that’s an ACOTAR ref </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hq5bwxu1153e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1gzxikf</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>new nail artist question!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzxikf/new_nail_artist_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1gzx6cq</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Hyperrealistic nails, I loved being able to do them 😁😁 I keep practicing to improve more and more💅😊</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/673swogms43e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1gzx103</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue and silver manicure and pink and black pedicure </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzx103</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1gzw84o</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Where do I start?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzw84o/where_do_i_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1gzvpdr</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>amazing nails done in vietnam for ONLY $38.55!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzvpdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1gzvyhj</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>A couple sets I've done recently</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzvyhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1gzvvqo</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Christmas Nails (self done)</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kyh99gqi43e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1gzvsp5</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunrise on a snowy day vibes </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzvsp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1gzvpm8</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp4qprogh43e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1gzvpho</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Favorite “watch me work” videos on clients?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzvpho/favorite_watch_me_work_videos_on_clients/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1gzvi1g</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Acetone and Movine</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzvi1g/acetone_and_movine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1gzulh0</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[YN] Gel Mystery Box Swatches! (Cream Clays) </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03rzfsmd943e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1gzufdt</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>What kind of nails do we think your prototypical “lady CEO villain” would have?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzufdt/what_kind_of_nails_do_we_think_your_prototypical/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1gzuczq</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>The length of my nails is natural and the white gives it an incredible touch, what do you think?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/potna4o9743e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1gzuadx</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Nail Breakage in Dry Climate</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzuadx/nail_breakage_in_dry_climate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1gzthiz</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>I know we're in november but some halloween ones id forgotten about! (inspired by @knixves on tiktok)</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzthiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1gztzdj</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Self painted 2 days ago</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/071uy7b4543e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1gztrrl</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Snowy nails for "winter"</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzbftzal343e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1gztr74</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>🖤⚫️🖤⚫️</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gztr74</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1gzt5nv</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need some shaping advice, my middle nails always look bulbous from the top view, but my sides are super straight? </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzt5nv/i_need_some_shaping_advice_my_middle_nails_always/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1gzt4zd</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Fall themed press ons for Thanksgiving!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzt4zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1gzt0wp</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Can never go wrong with basic french! All time fav🎀</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1v7k47by33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1gzsxa2</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is Glitterbels Unbelievabel Gel a hard gel? </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4pdj5jlx33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1gzsgeu</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>It's giving Umbreon</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwvw4lr8u33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1gzrj4h</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Eras tour x Christmas nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzrj4h/eras_tour_x_christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1gzrn1v</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 💅🏼 tech is just amazing </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzrn1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1gzrmoq</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>New nails inspired by Taylor Swift</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzrmoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1gzric5</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Scales on natural nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08l6gldin33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1gzqibu</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Help me decide</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzqibu</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1gzpfgp</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter nails </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzpfgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1gzq932</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Will a Nail Salon Be Ok if I Provided my Own Nail Polish?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzq932/will_a_nail_salon_be_ok_if_i_provided_my_own_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1gzq21y</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>DIY iced chocolate donut nails 🍩</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y11rg4e2d33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1gzoq8t</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Doll Nails 💅🏼🍓</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzoq8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1gzopoh</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Dip manicure yesterday. She kept knicking my cuticles with the drill bit. Today my nails are sore. Does this happen to anyone else? I'm getting fed up and at the point of DIYing my own nails.</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaspu83r333e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1gzofy5</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Fall nails</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzofy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1gzo5q6</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">finally found some motivation to do my nails again🥲🎉 </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpmfjzpsz23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1gznoun</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND black licorice. Loving this color with my ring 😍 </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apfbi7eqw23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1gzn9ph</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>First Russian Manicure ✨</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n55blsyrt23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1gzmwo5</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My nail tech popped off 💅🏻💞</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqtw3yc6r23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1gzml94</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black nails forever </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m77lggxo23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1gzmif3</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Jelly Gel Recommendations Plz</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzmif3/jelly_gel_recommendations_plz/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1gzm4l8</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Colorful Ostrich Design 💕</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9r01w1oll23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1gzhe1f</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Why am I getting scratches on my nails even though I’m waiting at least 20 minutes before touching anything?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzhe1f/why_am_i_getting_scratches_on_my_nails_even/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1gzfydz</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>HEMA free japanese gels</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzfydz/hema_free_japanese_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1gzlz8a</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>I’m going to be doing lots of reds and greens in the next few weeks, so I went with navy this week!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzlz8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1gzlege</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My fav set !!!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzlege</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1gzldwv</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>stars</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzldwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1gzl6bq</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>I did this with eyeshadow :)</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzl6bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1gzl5oq</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done like a turkey 🦃 </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e2qsrn9e23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1gzkxdk</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do think of my newly done nail? </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sd47w5dc23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1gzkte7</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>ladybug nails</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dk6lhwkb23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1gzkjqg</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl9vw1lh923e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1gzkd2f</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cancer risk with shellac? </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzkd2f/cancer_risk_with_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1gzkbz4</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>My Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzkbz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1gzjunb</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Polish over gel?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzjunb/polish_over_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1gzjpil</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Wicked 💚🩷</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzjpil</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1gzjpi4</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>In love with my fall nails</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzjpi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1gzjmue</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>OPI Trailglazer Press Ons</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtntrdxz123e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1gzjhu4</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>My dip glitter is soooo uneven 😞tips for dip powder plzzz I know it just takes practice too</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzjhu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1gzj5s0</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Got my nails done today! :)</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzj5s0</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1gzj1um</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Thanksgiving Nails</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzj1um</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1gzif78</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Beginner tips</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzif78</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1gzidld</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my favorite designs </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzidld</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1gzhx7n</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long time no nail </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzhx7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1gzhdii</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Blue marble 🌎</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmrpiphpg13e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1gzgxg9</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Dark blue is my new favorite 💙</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vaame4thb13e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1gzf38q</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>BIAB already peeled off after less than one week</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gzf38q/biab_already_peeled_off_after_less_than_one_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1gzeo3x</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using polygel </t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsvx1krvi03e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1gze7ao</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Advice on how to start doing my own nails?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gze7ao/advice_on_how_to_start_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1gze3gw</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press Ons for Friendsgiving </t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdr7gmz3b03e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1h06cda</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Help remove false full tips</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h06cda</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1h053dv</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Help healing and growing out my nails</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h053dv/help_healing_and_growing_out_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1h04trn</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>my first go at DIY appliques: added a Keroppi face to my green mani!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h04trn</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1h03xmn</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Quick dry top coat (QDT) question</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h03xmn/quick_dry_top_coat_qdt_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1h02znk</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Issues with Lucky 13 Lacquer - This Game Blows (Nov PPU)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0zma1br663e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1h02v31</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>I had high hopes for an elegant glowy look (and easy 1 coat application bc jts late and I’m tired) and the staining on my nails ruined it 😭</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h02v31</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1h02qfg</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>⛷️🌲❄️ ORLY Winter 2024 Collection - Après Ski (Color Pass Review)</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h02qfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1h0233z</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Winter Blue</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0233z</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1h02337</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Dupes for Essie Sugar Daddy?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h02337</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1h01lz5</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Late fall/Thanksgiving mani 🍂 🍁 </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h01lz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1h01cnt</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>So pretty!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h01cnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1h015o7</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Captured the rainbow of Aquarius (LynB Designs)</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50e11ytup53e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1h00buz</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>{PR} Meet Façade by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h00buz</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1gzzr8x</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Christmas toppers?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzzr8x/christmas_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1gzzdbb</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>What are your favorite glitter + shimmer polishes</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzzdbb/what_are_your_favorite_glitter_shimmer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1gzywsh</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Recs for nail art brushes?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzywsh/recs_for_nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1gzxdog</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Round base magnets... Any luck?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t67vb6h7u43e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1gzwwy8</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">25+ years of nail biting - I started painting my nails about a month ago. Safe to say I've stopped biting my nails for good! </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzwwy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1gzwm5m</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>i just love this pink so much!! ooo</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzwm5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1gzwdxj</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Shiny! ILNP Lily</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzwdxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1gzvabf</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Random question but what should I wear for my trip to the Grand Canyon?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzvabf/random_question_but_what_should_i_wear_for_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1gzv3y3</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aimed for Wicked ended up with a Christmassy Arcane </t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1ay2zq4d43e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1gzuzmy</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[YN] Gel Mystery Box Swatches! (Cream Clays) 💅 </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evomrl15c43e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1gzuota</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Powerslide ✨ </t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzuota</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1gzugu2</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Lazy reflective blobs</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzugu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1gztwti</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>My Olive Ave collection! Love them</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp67ss7m443e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1gzthka</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Psilocin owners, help!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzthka/psilocin_owners_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1gzsj0s</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is my nail wavy? </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33o1xcuqu33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1gzry8w</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Golden Sky feat. Fool's Gold</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzry8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1gzrtc3</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Pour one out for my forefinger 😩 usually paint my nails at home but I couldn’t bring myself to cut them lol</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzrtc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1gzqw08</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Feeling fancy 💗🧚🏾</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzqw08</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1gzqvbe</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>A press on set I did for christmas</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gtf4gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1gzqola</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>concert nails</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzqola</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1gzqlpj</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>My current fav is a magnetic, linear holo, gray jelly</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fpzz77itg33e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1gzq22h</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani - take 2 🦃</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzq22h</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1gzq1lq</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Faux Spirit</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wsxuxvzc33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1gzppae</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Polish starts thin and quickly becomes thick WHILE using but will be thin again if I use it another time</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzppae/polish_starts_thin_and_quickly_becomes_thick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1gzpfw7</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>PPU Wrong Items</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzpfw7/ppu_wrong_items/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1gzpa5m</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November Manis </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzpa5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1gzotfv</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Stolen pics?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzotfv/stolen_pics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1gzokxy</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Luna 💫🌙✨</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzokxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1gznz9w</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>holly nails</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wugptavny23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1gznrfl</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hush v Root of All Evil? </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gznrfl/hush_v_root_of_all_evil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1gznm49</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Not perfect, but what 4 months of hyperfixating on nails does to a gal lol</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmpezel7w23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1gzncxg</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funky fall mani </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzncxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1gzmrcy</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>These sales are my downfall</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzmrcy/these_sales_are_my_downfall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1gzmqrh</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Lacquergram: How can I share my collection with someone not on the app?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzmqrh/lacquergram_how_can_i_share_my_collection_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1gzml29</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my favorite (and cheapest) polishes </t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21xfwg7vo23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1gzmfk8</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Early Christmas nails</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1x9gbqsn23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1gzme8z</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mood Ring velvet </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y6f2wvvin23e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1gzm527</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Showdown of dupes, destashed both</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn8io87pl23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1gzm4fu</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>small but deadly…🥲</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5h5gzekl23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1gzlvek</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Love my nails but I wish I was better with the magnets</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vr1ybanj23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1gzlfwk</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Looking for a UK-based copper shade</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzlfwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1gzlcnf</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Two weeks with no top coat using Bluebell</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y5470eonf23e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1gzl9f1</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First indie polish nostalgia </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzl9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1gzl76v</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Skittling my way through untrieds because I'm indecisive 😝</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzl76v</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1gzkk7s</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time having chocolate 🍫 </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v5zhznl923e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1gzkju7</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm thankful for purple </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzkju7</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1gzkhy7</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Inspired by changing leaves</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7v0oky3923e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1gzke53</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>NO ONE MOURNS THE MANI</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzke53</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1gzkdwj</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Press-ons? </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzkdwj/best_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1gzkcl9</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Early Christmas skittle feat. my very sleepy (and annoyed) cat</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzkcl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1gzju1o</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Nail question</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzju1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1gzjn7x</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Wicked 💚🩷</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzjn7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1gzjfyr</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>“Fluer-t” by Sally Hansen Color Therapy (111)</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aejof0cf023e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1gzixqn</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Can someone help me identify names of these China Glaze polishes?</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzixqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1gziq0o</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joining the Wick nail trend </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arptexc2u13e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1gzimyi</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Jinx Arcane inspired nails - this was my first time ever doing my nails so please ignore the wonky application</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weqsp7wxs13e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1gzhzug</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Get jinxed! (Arcane inspired mani)</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzhzug</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1gzgx05</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Cut them short(er) after having long nails for a while 🌸</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzgx05</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1gzge7p</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>More adventures in horseshoe magnets...</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzge7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1gzgc59</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzgc59/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1gzg6cb</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hema free japanese gel? </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gzg6cb/hema_free_japanese_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1gzfzs5</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">'We have mooncat at home' </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzfzs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1gzftb3</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>My Last Haul Until September (at least)!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/livzvalz703e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1gzef1z</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Any recommendations for a light blue jelly nail polish with sparkles (and I mean A LOT of sparkles)? Something like in this pic</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xczsa9ocf03e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1h06qtq</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>post in the car got taken down but i really love this set ! 🪬🩵</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h06qtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1gzznpg</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Sea Floor🏝️</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a4xw9tazc53e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1gzwz59</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello Kitty Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuamz1k1r43e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1gzwx9o</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Thanks to you amazing people, here are some sets from orders she got!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzwx9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1gzw0vb</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fall nails from October </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzw0vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1gzugps</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Princess Luna hand-painted</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hryj3woj843e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1gzt1hi</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Winter wonderland ❄️☃️</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzt1hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1gzswff</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How fun are these </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ofooq5fx33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1gzqig7</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Looking for some advice</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gzqig7/looking_for_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1gzpnr6</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>I love to innovate with my nail designs! 💚👽</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ghx77wba33e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1gzoukh</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>The most demure set I've done on myself ✨🍰☕🫖</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzoukh</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1gzoh96</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>fall nails</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzoh96</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1gzmtfr</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I’ve got 10 million hand-me-down Beetles Gel Polishes and a Dream</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzmtfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1gzmccn</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>My new nails, Beautiful</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gzmccn</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1gzm4br</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Colorful Ostrich Design 💕</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkc3gkljl23e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1gzex89</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>first time using hard gel! need advice.</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv77g14am03e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov 27 08:11:33 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_01.xlsx
+++ b/data/collected_data/2024_12_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C492"/>
+  <dimension ref="A1:C687"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8798,6 +8798,3321 @@
         </is>
       </c>
     </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1h0yw7q</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[Acrylic] Can I glue on just the nail tips at home, then go to the salon and have the nail technician apply the acrylic over? </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0yw7q/acrylic_can_i_glue_on_just_the_nail_tips_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1h0y2qu</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>My Christmas plaid pressons🧣</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0y2qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1h0xnof</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Vacay nails for Cabo ! 🇲🇽🍹🏖️</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0xnof</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1h0xmf8</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do your gelx nails last as long as acrylics? </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0xmf8/do_your_gelx_nails_last_as_long_as_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1h0weav</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>my fantastic mr fox inspired nails</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0weav</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1h0x500</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>I’m really loving theses nails!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfr91zqsrd3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1h0wupd</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Questions about nail salons from someone with contamination OCD</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0wupd/questions_about_nail_salons_from_someone_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1h0wod9</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Love my nails 🌸🎀💗🩰</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjnbk3vqmd3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1h0wgct</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on the ombre nails. </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0wgct</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1h0w00f</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Festive nails !</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qefuywwfd3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1h0vkw3</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Nail day!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk9wcautbd3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1h0vff7</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Thanksgiving Nails</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0vff7</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1h0val8</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>turned out cuter than I expected 😍</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/130kt8f19d3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1h0v7d9</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In between holidays set </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdmdmt068d3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1h0ua01</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Bliss kiss nail oil</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0ua01/bliss_kiss_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1h0ur3p</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Its lilac but looks royal blue on cam. Thought i did pretty good this timee, been messing them up latelyy, I suck at getting the sides and the nail bed clean. Second pic is true color</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ur3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1h0uv1h</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>I have made an Arcane Shimmer Nail! 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zfdkc48w4d3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1h0u9ar</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Nail Extension too small - what now?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0u9ar/nail_extension_too_small_what_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1h0tsxk</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>WhimsiGoth Nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8y8k8pwuc3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1h0tirp</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel nail journey </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0tirp</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1h0tgzm</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>eyes</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6m0lofvrc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1h0tdnf</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>my tech was so excited for his first winter set of the season</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0tdnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1h0r017</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Do we likeeee? I’m queen of second guessing myself.. but I actually really love them!! What do you think!?🤎</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0r017</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1h0tb0d</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something new </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxcpegddqc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1h0t7h7</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Green cat eye</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l61ghltipc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1h0t4mc</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>I love xmas nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7jrvkqsoc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1h0ssau</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Finally did one more set on myself before my induction tonight! Can you guess what I'm having? 😅</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zomysopmlc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1h0ss6b</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Found these around Halloween time and felt they were perfect for going to see Wicked</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg6mfegllc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1h0rk03</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set — Color choice feedback? </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6ms6wguac3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1h0rad9</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0rad9</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1h0r969</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Shein press on nails! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0r969</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1h0r2rt</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Red and Gold. I love it 🥰</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugtekbkr6c3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1h0q9vv</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Loving this look</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqotmp900c3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1h0pz22</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>X-Mas Practice Set</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj0ghgakxb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1h0pxwp</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>DMB Nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0pxwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1h0pt32</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Florals! </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0pt32</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1h0ppyn</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Calico set for the fall 🍂</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ppyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1h0ple8</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>I loved doing this Miffy holiday set on myself! Would you get it? 🤭❄️✨</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ple8</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1h0p4d6</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>What a beautiful design 😩✨</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huej74roqb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1h0ozzf</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Gift Help</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwtr077tpb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1h0ohmj</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Very happy with this eclectic (?) set!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mniak9iulb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1h0o9as</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Newbie looking for suggestions what would look good with my nails for an engagement shoot</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0o9as</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1h0nzri</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New press ons 🌺 </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0nzri</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1h0mpnq</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Should I cut this nail? Will it regrow normally on its own?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vftp0krl8b3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1h0na2f</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>How to make press on nails less transparent?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjd77aeucb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1h0n4c5</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Self-taught Gel-X</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0n4c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1h0n3gy</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Take a trip down candy cane lane with me! </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0n3gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1h0mue6</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>New set 💕✨</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0mue6</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1h0mh2l</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>My Fall &amp; Thanksgiving set!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0mh2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1h0lpkg</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>First time getting 3-D/freestyle</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hu5fiw481b3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1h0khjy</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>anxious to go to an at home nail tech?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0khjy/anxious_to_go_to_an_at_home_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1h0ktnk</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do nail salons actually help nail growth? </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9aqbjbvua3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1h0kjnz</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Former nail biter…</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0kjnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1h0kjin</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Christmas nails! 🎄</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0kjin</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1h0kfw9</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Festive Mushrooms 🍄🌲</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt394275sa3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1h0kde5</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Just in time for Christmas. Gel-X Red</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0e6y1amra3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1h0jv5p</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">recommendations and advice </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0jv5p/recommendations_and_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1h0jwpa</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Back to my old ways</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azdkxouboa3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1h0juzf</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New designs </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0juzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1h0ji3i</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 month progress </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ji3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1h0iuxe</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I ask for at Nail Salon? Inspo pics credit @pheobelilyfall on pinterest </t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0iuxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1h0iizy</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Winter's gnome set - I am so not inspired by this season...😒</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0iizy</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1h0ilnk</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Concert and birthday nails</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ilnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1h0irr0</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>First time with press ons. Do they look weird?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0irr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1h0io8a</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>forgot to post this manicure before taking it off :3</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0io8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1h0iev7</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Going on vacation for a week but can't have anything on my nails when I come back</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0iev7/going_on_vacation_for_a_week_but_cant_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1h0hvt2</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Nails feel so weak after biab/acrylic</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0hvt2/nails_feel_so_weak_after_biabacrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1h0hn65</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>i love these sm &lt;3</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx8srm4d8a3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1h0hfj3</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my natural nails </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0hfj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1h0h64g</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>How do these look?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqgkdkux4a3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1h0h62q</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>🩷🤍🩷🤍🩷🤍</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0h62q</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1h0gs7j</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>My Anatomy themed nails</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0gs7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1h0gnob</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never too old to have a bit of mermaid in your life 🧜‍♀️ Cre8tion gel mermaid polish in shade 1. One coat of black gel underneath, Two coats of mermaid. </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggjk3nm81a3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1h0g8kt</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question RE: French tips </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4wr7fh4y93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1h0fcs0</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Guess the fake! I broke one and had to use a fake one. Can you guess which one it is?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugjtgflnr93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1h0g7up</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cut or Keep? </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0g7up</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1h0fjp7</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">look at this nail polish I had neglected for years! </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6nj1j092t93e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1h0fh6c</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting my nails done </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn9x7bvjs93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1h0f6ke</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>My new manicure 😻 Not too wedding- like?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p7wtfmfq93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1h0f26k</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Water based nail paint</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0f26k/water_based_nail_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1h0ewx2</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Not cooking but still serving</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ewx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1h0ess2</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass Slipper ✨ </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ess2</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1h0esbk</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Cloud-colored nails</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w1afs1en93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1h0epse</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>I just did my first set of acrylics!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpli80nwm93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1h0eood</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>🐝🍯 Honeybee Nails 🍯🐝</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh1xl79om93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1h0dbfb</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did I do? First time press-ons </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0dbfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1h0bfix</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Barbie / Power Puff inspired✨💖</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0bfix</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1h0edgj</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Sharing progress🖤</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0edgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1h0e1u4</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Finally time for Christmas nails</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0e1u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1h0dr03</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>How to DIY nails for 13 year old</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0dr03/how_to_diy_nails_for_13_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1h0dqkt</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Repair or leave alone?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0dqkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1h0dclt</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Squad plus Essie = Awesomeness </t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0dclt</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1h0dbsy</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Damaged Nail beds </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0dbsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1h0d8rc</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>🤍❄️✨</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xutifqbb93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1h0d7au</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Longest my nails have ever been….</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0d7au</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1h0cqbs</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Some Holiday(ish) Nails</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0cqbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1h0c93t</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting your nails done is such an amazing feeling ✨️ </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buqxps03393e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1h0c7n9</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Monday night nail art ☠️🌹</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onbjdofq293e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1h0beny</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails By Annie </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h0beny/nails_by_annie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1h0amm4</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got this set today. Acrylic nails and gel polish. </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5uy3279o83e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1h0ytvw</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Green Polish with a Pink Topper looks so good 💚🩷</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ytvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1h0yff2</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>One day I'll get them</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0yff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1h0yeiw</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Is this legit? Does ILNP actually have an Etsy?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ocn8wp66e3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1h0wh1m</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>attempting to cram some late-night work in.. keep getting distracted 🤩</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0wh1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1h0w5lu</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sims 4 Life &amp; Death themed mani 🦋🪦💀 </t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0w5lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1h0w0jy</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Lava nails</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0w0jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1h0vr8m</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Why are black nails so sexy 🙃</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwrtibkidd3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1h0v281</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>LynB Fair Isle 1 vs 2 Coats</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0v281</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1h0unf3</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Polish cracking ??</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0unf3/polish_cracking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1h0uab1</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Bliss kiss nail oil</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0uab1/bliss_kiss_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1h0u8y6</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>My favorite part of the weather cooling down!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qw1ykm1zc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1h0te4z</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>sally hansen hardener or strengthener?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0te4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1h0t7xy</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Diy dupe for Cuticula, Creepin it Real</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0t7xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1h0t6ou</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Snow like polish with holographic micro flakes?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0t6ou/snow_like_polish_with_holographic_micro_flakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1h0t3e9</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>The perfect fall orange chrome</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0t3e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1h0sypb</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Wicked Nails</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0sypb</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1h0rs4j</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Polish like this one that’s NOT sheer?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0372ljscc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1h0rjgv</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know what causes this? Details in comments </t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0rjgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1h0ra8t</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>DMB Nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ra8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1h0r5zf</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Our Laughter Carries on a Warm Wind…at the airport</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0r5zf</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1h0r5v6</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>november’s nails 🍂🍎🦃</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0r5v6</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1h0r175</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first magnetic polish did not disappoint </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0r175</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1h0qfpb</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Londontown Instant Smudge Fix</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0qfpb/londontown_instant_smudge_fix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1h0q569</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>How many times do you wrap your tip with polish?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0q569/how_many_times_do_you_wrap_your_tip_with_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1h0q2sp</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Dupe for Lumen’s Shimmering Moss?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adift9seyb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1h0ostm</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">head in the clouds + fairy dust </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qa10hr8ob3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1h0o89c</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>LynB Designs is so good!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcjtmc7wjb3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1h0ni0w</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Thanksgiving Nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ni0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1h0nhyi</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>New to this, but loving it!</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyhvkchfeb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1h0nd90</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clionadh lives up to the hype </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/31u899igdb3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1h0nbtm</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall skittles mani </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpvhufq7db3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1h0n7zc</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>PSA: read your bottles when you paint so you don't accidentally use a peel off base for your top coat...</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0n7zc/psa_read_your_bottles_when_you_paint_so_you_dont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1h0n5fx</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Novice - Dry Time? </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0n5fx/novice_dry_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1h0mgsl</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pooping after polishing </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0mgsl/pooping_after_polishing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1h0m0li</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Contact dermatitis from gel saved my nails</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0m0li</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1h0lx1h</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>There's an L.A. Colors Advent Calendar at CVS</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0lx1h/theres_an_la_colors_advent_calendar_at_cvs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1h0lku2</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Wanted to channel autumn</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/snzaumi80b3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1h0l9jn</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A THANK YOU to this subreddit for crucial information about gel allergies </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0l9jn/a_thank_you_to_this_subreddit_for_crucial/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1h0l8xz</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails 🦃</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqzzverwxa3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1h0l5sg</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally swatched my polishes! </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjqzm8zbxa3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1h0kr4q</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Witch Hazel</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0kqgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1h0kp73</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall/Thanksgiving Skittle </t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0kp73</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1h0koi4</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>SO. GOOD.</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0koi4/so_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1h0jgwy</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>I love you more than all the stars in the sky ✨</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hafypo6la3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1h0j1vd</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Dupe request for CC Terrior</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dibkrpm8ia3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1h0i272</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>🎮Playstation Controller🎮</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0i272</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1h0hwu0</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>One trend I’ll forever be obsessed with is deep vampy red nails 🍷</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl1w0c6aaa3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1h0h977</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Dupes for Polishes from Lights Laquer</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0h977/dupes_for_polishes_from_lights_laquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1h0h2db</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tragedy struck! What color will minimize the short nail or should I cut them all back? </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiijs3q64a3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1h0h0dp</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Storage recommendations</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0h0dp/storage_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1h0g7sj</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat question </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0g7sj/top_coat_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1h0g1dv</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Pink &amp; blue is my fav color combo</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0g1dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1h0g12k</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I allowed to be dissapointed? </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxmgtsglw93e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1h0ftjm</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Holo skittle for fall 🍂</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ftjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1h0fohx</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Idk why I waited so long to try Marsala Jelly! She really is *that polish* </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0fohx</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1h0fec7</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for Ethereal’s Shell Phone</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0fec7</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1h0f3vl</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>What’s the best non-gel magnetic polish?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ek415gvp93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1h0ex7t</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Organized my collection by color!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ex7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1h0ep37</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Working nights makes it hard to make salon appointments. Decided to take matters into my own hands.</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n749d62rm93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1h0e2p4</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Playing with some low budget polish</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0e2p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1h0dzsq</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I apply nail powder over the polish? </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1deboztch93e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1h0dmvf</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Stamping over Dazzle dry help</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0dmvf/stamping_over_dazzle_dry_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1h0d9bv</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Squad plus Essie = Awesomeness </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0d9bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1h0co44</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I’ve never raked so many leaves in my life 🍁</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qbftwqj693e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1h0c4t5</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle/Proximal fold help </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0c4t5/cuticleproximal_fold_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1h0c1k2</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Psilocybin is bonkers</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fl2b0cna193e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1h0bn0u</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>How can I put together a Nail Polish kit for a Christmas Gift?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h0bn0u/how_can_i_put_together_a_nail_polish_kit_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1h0beyy</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>I don't know what vibe this is but Im feeling it lately</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0beyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1h08lx3</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>too excited with this set so i want to show it to people :x</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h08lx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1h08htl</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>BKL (Bees Knees Lacquer) Divine Mortals Comparison post</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h08htl</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1h0yy6z</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>black&amp;nude gel-x!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f41xl9wsce3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1h0xrdp</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love pink </t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnt0kgwkyd3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1h0vuac</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0vuac</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1h0v5c1</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Wanted to do my nails before thanksgiving 💅</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0v5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1h0uykp</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I have made an Arcane Shimmer Nail! 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c8enundt5d3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1h0sz67</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Dipped in metal for my birthday by @kalsrebelliousnails</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0sz67</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1h0sudu</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>✨💖✨</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/djo4ufx4mc3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1h0ppof</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>new to nails</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ppof</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1h0ofy0</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Another (imho) great set by my nail tech</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gcgs1gilb3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1h0obob</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Are you ready for a peaceful Christmas season?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0obob</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1h0o1du</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Why do my nails get matte after top coat?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h0o1du/why_do_my_nails_get_matte_after_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1h0nc35</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>A couple more sets that clients have ordered!!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0nc35</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1h0la5j</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this style and this is one f my fav colors </t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0la5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1h0ikpo</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Winter's gnome set - I am so not inspired by this season...😒</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0ikpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1h0gbtv</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Cow style model 🐄</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxh5bc0ty93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1h0f7pj</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>I loved this result</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m7h5weoq93e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1h0er2s</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>You like have XL, Large, Medium or small</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h0er2s/you_like_have_xl_large_medium_or_small/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1h0eo5t</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>🐝🍯 Honeybee Nails 🍯🐝</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5l1op1bkm93e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1h0capy</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>a little bit natural and modern without losing the style</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0capy</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1h0c5w1</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">deep blue! I'm improving my lines </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0c5w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1h0bf2w</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>How do my super mario press ons that I made look?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzo3z4yqv83e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1h0a3a9</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started playing with a framed cateye look </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0a3a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1h09qzm</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Magnetic polishes - do you magnetize the first coat(s) or only the final one?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h09qzm/magnetic_polishes_do_you_magnetize_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1h09pyv</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Sponge question</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h09pyv/sponge_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1h07qto</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Love this simple but gorgeous nails!!🌸 Nail inspo from Instagram❤️</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ictuw8fp73e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov 28 08:11:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_01.xlsx
+++ b/data/collected_data/2024_12_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C687"/>
+  <dimension ref="A1:C878"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12113,6 +12113,3254 @@
         </is>
       </c>
     </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1h1qzd9</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Very proud of my natural nail progress since September 🥰💅</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1qzd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1h1qi04</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Winter wonderland done by meeee</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1qi04</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1h1pbue</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first ever set on human hands! second ever set total, thoughts? </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1pbue</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1h1pscg</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Finally hopped on the band wagon!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1pscg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1h1prkx</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday joy! </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pqs10jam6l3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1h1p473</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>The white part of some of my nails are shaped weird. Is this permanent or will it round out eventually?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfc1lda7zk3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1h1ou02</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Grinchy Green nails</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1ou02</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1h1onf5</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>is sparkly nail polish seen as more childish/less professional than solid colors?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1onf5/is_sparkly_nail_polish_seen_as_more_childishless/</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1h1of95</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Got the winter blues</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9wmx13lrk3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1h1nvka</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emerald chrome nails for Wicked! 💚 Gel extensions! </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7jkya9vlk3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1h1n4as</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>A lil thanksgiving theme</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1n4as</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1h1mxga</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November nails </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1mxga</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1h1mswd</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I'm loving these deep jewel tones! They're kind of giving me maple and blackberry syrup vibes 🍁🍇🥞</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr6smwysak3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1h1mh7x</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love these!i </t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1mh7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1h1mcym</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Which brand to buy?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1mcym/which_brand_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1h1m6y5</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>New set 💚❄️🌲⭐️🪴</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pikuoj0q4k3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1h1l2vc</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>What is going on in the gel nails community….</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1l2vc/what_is_going_on_in_the_gel_nails_community/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1h1lxa2</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help for choosing UV/LED lamp. </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1lxa2/need_help_for_choosing_uvled_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1h1lqw1</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>I asked for Snoopy, bread, browns and plaids and my nail tech delivered 🤎🥖🥐🍞</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1lqw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1h1lhhg</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>I know people aren't always impressed with long, natural nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqdzwdtxxj3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1h1lh85</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">lil 3D abstract gel-x set i did for my sister </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/day6k4ewxj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1h1lbpj</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Is this normal for gel nails?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1lbpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1h1l8s9</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Start of Christmas nails. </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf5gk7apvj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1h1kvns</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My first try :)</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1kvns</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1h1jqz4</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how do you guys floss </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1jqz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1h1ko3w</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweata Weatha </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1ko3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1h1kmnn</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Damaged nail?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ioz5oytpj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1h1khsc</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Fall press ons</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbu0vobjoj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1h1kge9</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>First set</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1nnfgm6oj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1h1kb2n</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>birthday nails🖤❤️🩶</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1kb2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1h1j456</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 1 month nail journey! </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1j456</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1h1hgeo</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Removing cuticles</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1hgeo/removing_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1h1jjsk</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nyofyivfj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1h1jjb0</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>just did my other hand for the first time !</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5c9vp23tfj3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1h1isd9</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>My gelx nails keep popping off.</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1isd9/my_gelx_nails_keep_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1h1if4g</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French tips and gel polish </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1if4g/french_tips_and_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1h1iarf</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Thanksgiving Nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m5n01t25j3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1h1i7xo</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Can’t decide if I like this color</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx5anx4e4j3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1h1hw4f</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wife said new ring, new nails! </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1hw4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1h1hmr3</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter nails in the house </t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iub4znwhzi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1h1h16p</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+nails for my wedding</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5d6trtjui3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1h1ggk0</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Detached nail </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlxa4tf4qi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1h1gnne</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>First time in months doing Acrylics 😫🫶🏼 Her anniversary and some Christmas themes 🥹💕</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1gnne</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1h1gj2u</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍂🧡 One last Autumn mani 🦃🍁 ILNP Harvest skittle </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1gj2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1h1gfob</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Different shape nails? Can this work?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd6yrmdxpi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1h1g62h</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Trimming GelX</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1g62h/trimming_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1h1eiox</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>How’s this shape?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvcwbrczai3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1h1bri2</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I heal this while also protecting it from myself? </t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1bri2</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1h1enxh</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>When a nail breaks off at the base, how do you preserve the skin growth?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1enxh/when_a_nail_breaks_off_at_the_base_how_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1h1etcn</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You’re the Sunflower 🌻 </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1etcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1h1fakf</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>I think I might be getting engaged Friday. Should I have my nails redone?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eef5ndb0hi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1h1fcg0</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Acrylic nails by me!!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1fcg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1h1f98q</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Feeling very Elphaba &amp; Glinda 💞💚</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh51jmrpgi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1h1f6zh</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1f6zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1h1erft</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Got rid of the gummy bears cuz they were too tall for my wedding ring (lol)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgxsvv4vci3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1h1enw9</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>What do you think about this blue?💙</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1z4i5h3ci3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1h1ebbq</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Are they seasonally themed? No! Do I still love them? Yes!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1ebbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1h1ajfe</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to stop touching my nails! </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1ajfe/how_to_stop_touching_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1h1ae18</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Bruises from acrylic removal from a salon</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1ae18</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1h1a9xs</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>another artist for a fill?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1a9xs/another_artist_for_a_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1h1c0qi</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown discoloration under nail </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pmc5ol1sh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1h1df3k</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye Christmas trees </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xramwpk2i3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1h1de72</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Gellac Peel-off </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1de72/pink_gellac_peeloff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1h1cwkc</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Loving these fall nails!</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7reuhgoyh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1h1bjer</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Finger tattoos on this sub</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1bjer/finger_tattoos_on_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1h1ay4w</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Back to DIY after a couple of years of getting professional manis</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1ay4w/back_to_diy_after_a_couple_of_years_of_getting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1h1aql1</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there a difference between luminary SET and just a luminary manicure? </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1aql1/is_there_a_difference_between_luminary_set_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1h1aibm</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Cat eye red to start the holidays 😻</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2ue4mczgh3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1h1aiax</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Longmaletoenails </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqgb3rl5hh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1h1ahjk</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>sheer butterfly nails 🦋✨️</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03962ni1hh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1h1abwk</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>New ice princess nails ☺️</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbxpbkdvfh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1h1a603</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Tipping your nail tech</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1a603/tipping_your_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1h19oxt</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some Walmart press ons painted over. </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm1gfsr3bh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1h19hef</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When Fall and Winter collide </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h19hef</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1h1936r</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All natural set perfect for winter </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1936r</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1h1919a</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>I love the nails she does @queen_nails_df</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m61q97u96h3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1h18bgm</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>what is wrong with my nails??</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h18bgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1h18860</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The perfect nude for me. </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h18860</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1h187nd</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>My acrylic  powder nail cracked and broke what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zesg9i30h3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1h183br</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Hey y'all first time trying to do acrylics, i know they're not the best but thought i'd share because i'm proud</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h183br</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1h17chs</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>I found the perfect fig color for this year</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47ojfdqitg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1h12i45</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I pulled an all-nighter before my Japan trip to do these. 🫴🏻✨</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h12i45</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1h171a2</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is gel overlay/builder gel better than shellac or acrylics? </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebdrclo5rg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1h16xxi</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>💙 Blue nail design 💙</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnvset0fqg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1h16v0h</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In growth and new color </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w89fo0cspg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1h16v0c</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Nails for the week. 💅🏾💖</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ixr4tdspg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1h16ghj</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>fishy nails 🐟</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2o6ddi7mmg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1h15sjj</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>GTD</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c9fc06ahg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1h15pf2</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>One of my favorites</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bysqrqjgg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1h15kgf</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple and classy, I love them! ♥️ </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af28y1nefg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1h15f8b</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have fat, stubby, Megan Fox thumbs. What would the best shape be for me? </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztfc9n77eg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1h155hf</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! What causes this? </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h155hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1h14vu8</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>First nail appointment must do's</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h14vu8/first_nail_appointment_must_dos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1h14f2r</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>What are some solid options for guys getting a manicure?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h14f2r/what_are_some_solid_options_for_guys_getting_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1h14ctb</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Best shape for typing?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h14ctb/best_shape_for_typing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1h13n02</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>First time doing ponties ✨</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1orhb4qyf3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1h139fd</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>👽💚</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8xxg680vf3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1h12wiv</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Need a replacement for OPI An Affair in Red Square</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h12wiv/need_a_replacement_for_opi_an_affair_in_red_square/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1h12rw1</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>That gold flake 🫦</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h12rw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1h12q2e</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally did a winter set 🧊💙 self-taught, hard gel </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h12q2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1h1r32h</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Ilnp - finalizing list</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62x8rqlwml3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1h1qnuq</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Using two magnets instead of a horseshoe magnet!🧲 </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i10jio9dhl3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1h1pw38</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">black friday cart draft, thoughts? </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq06kainrk3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1h1pjfd</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - I don't need luck, have ammo</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y64giddz3l3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1h1p2yw</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Subtly Depressed Thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvnqgqltyk3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1h1oz0a</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>I consider glitter a palate cleanser 💁‍♀️</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1oz0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1h1o1wt</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Classy Dinner</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1o1wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1h1nmar</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i was going to complain about the casualty but then realized i can see my red shirt reflected in my middle nail lmao </t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xmg4tj3jk3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1h1lokx</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Anyone else not post pics because you can't do the polish justice on camera?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1lokx/anyone_else_not_post_pics_because_you_cant_do_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1h1lant</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I have re-joined the nub club</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1lant</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1h1kuzz</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbhrz071sj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1h1kqc0</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finding Feathers Lacquer Black Friday </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1kqc0/finding_feathers_lacquer_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1h1kblb</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations for matte top coat? </t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1kblb/recommendations_for_matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1h1k263</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Thoughts on my ILNP cart and first ILNP order? Are Reign and Maiden Lane too similar? Any must-have scattered holos for someone who loves grays, blues, and greens?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eb9tln7kj3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1h1im6v</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Maybe I Need More Greens</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/repohb4u7j3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1h1ihzq</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Dragon Scales living up to its name and protecting my finger.</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1ihzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1h1hapn</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flower Child Skittle </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gdwgpjbswi3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1h1h5fo</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Im not really a waitress </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1h5fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1h1h31w</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Questions about acrylates in ridge filling base coat and regular nail polish</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1h31w/questions_about_acrylates_in_ridge_filling_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1h1gerz</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newb November show off </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1gerz</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1h1gby4</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍂🧡 One last Autumn mani 🦃🍁 ILNP Harvest skittle </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1gby4</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1h1g0aq</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Discovered a great combo 💚</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1g0aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1h1fjh3</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1fjh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1h1fe1y</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>What are the tips and/or products that have made the biggest difference in your polish game?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1fe1y/what_are_the_tips_andor_products_that_have_made/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1h1f1wy</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Impress no glue mani-help with removing adhesive</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1f1wy/impress_no_glue_manihelp_with_removing_adhesive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1h1ek1o</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Been waiting for weeks. I could cry 😭</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snimtk2abi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1h1eihw</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Studio Ghibli inspo</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqyv2jxxai3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1h1efg6</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Household-material mat for nail art?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1efg6/householdmaterial_mat_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1h1e6wq</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Layered my magnetic and shimmer holo PPU picks, with the thumb cat eye and the rest velvet style</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/94q16v4e8i3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1h1d7kp</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else watching the polish cap drama go down? </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aevo5y501i3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1h1cglb</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Sally Hansen Miracle Gel Replacement Brush?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1cglb</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1h1c475</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>ILNP Chai Latte vs Holo Taco Fifty Shades of Greige</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1c475/ilnp_chai_latte_vs_holo_taco_fifty_shades_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1h1bxxr</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ll never grow tired of the glowy finish </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1bxxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1h1bwyv</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Thanksgiving Prugly</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1bwyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1h1bduz</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>At what point in the manicure do you guys use KBShimmer's Smooth Moves?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opqgxw4knh3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1h1afif</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani ft. so many sparkles</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1afif</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1h1aec6</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snow and Sunshine </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72f4a4y7gh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1h1a36u</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are y'all using for DIY nail oil? </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0yszkt2eh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1h19r9t</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Nailfluencers with dark skin</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h19r9t/nailfluencers_with_dark_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1h19qsb</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Me a couple weeks ago: "I can't justify buying yellow nail polish, it's unflattering and I'll never wear it." ...Now me literally yesterday: "💛✨️"</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h19qsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1h199s6</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was only going to buy from ILNP this Black Friday… </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wftlfq0x7h3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1h188w0</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deck the halls with boughs of Hauly 😂👌🏻 </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd3mc87d0h3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1h187u2</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with these stained glass nails </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdguzq350h3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1h17zwm</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pitting in polish? </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efs273lfyg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1h17vxf</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Can someone please help me find this color?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ognd6nxmxg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1h17t7w</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>I am thankful for this nail polish ✨</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8bjl8f42xg3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1h17m03</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Blurring base coat without PVB?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms6mm77mvg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1h17i3e</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>BKL comparisons</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h17i3e/bkl_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1h17huz</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Any go to polishes for gifting?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h17huz/any_go_to_polishes_for_gifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1h17gkk</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>From my Night Owl Lacquer BF haul</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h17gkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1h16szu</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>☀️Sun God: Ra☀️</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h16szu</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1h16h91</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Purple ✨</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kes1csrmg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1h16f5h</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>fishy nails</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sap402hbmg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1h15n79</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Applejack from Nov PPU</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43wnj1e1gg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1h15by4</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I have one hot finger on each hand.</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h15by4</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1h158s8</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Recent favourite crème/layering polishes?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h158s8/recent_favourite_crèmelayering_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1h153wp</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! What causes this? </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h153wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1h14v2w</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Nail Wrinkling Help</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h14v2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1h14pyf</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Win Big - Revlon Colorstay alternative.</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h14pyf/win_big_revlon_colorstay_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1h124xg</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>These are the polishes I plan to wear in December.</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx5bnufmif3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1h11md0</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>ICY GRL ❄️</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h11md0</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1h116cf</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Layered polishes for the first time!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj43umhm6f3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1h0c95z</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Difference of a year</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38qlgbzwa03e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1h0nfn0</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>My Wicked/Oz Skittle!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0nfn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1h0skk7</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aio5cmqqjc3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1h0zk8r</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Finally nailing this fake water marble thing</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0zk8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1h0zivx</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>November manicure review 🍂</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h0zivx</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1h1qjol</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Winter wonderland!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1qjol</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1h1nv3z</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>so happy with these!!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1nv3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1h1mhsr</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bedazzled </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q5c7hwn7k3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1h1igf3</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>My Christmas set☃️</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1igf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1h1go01</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>First time in months doing Acrylics 😫🫶🏼 Her anniversary and some Christmas themes 🥹💕</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1go01</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1h1gi6u</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>SailorMoon Nails</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09kc8l3hqi3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1h1g4eb</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Corporate holiday party nails</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1g4eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1h1g1ex</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time hand painting flowers </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1g1ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1h1d7g4</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">improving my technique and this is my fav color so far </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1d7g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1h1ay0r</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Nail art with only polish</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1ay0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1h1au9x</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>help with eyeshadow ombres T-T</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h1au9x/help_with_eyeshadow_ombres_tt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1h1afg4</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>sheer butterfly nails 🦋✨️</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7mdkxylgh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1h1a9n9</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Decided to be creative with black</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qhk6qmkeh3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1h184l0</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I made my mother's nails, she is my perfect canvas</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti1y40bbzg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1h17f8q</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Base Coat for Stickers</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h17f8q/base_coat_for_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1h173j8</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LADY GAGA DISEASE NAIL ART </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h173j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1h16xyb</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>God of War Nail Art</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kbz0codqg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1h16xg0</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>💙 Blue nail design 💙</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auss5robqg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1h16phi</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>𝙂𝙃𝙊𝙎𝙏𝙁𝘼𝘾𝙀 𝙎𝙉𝙊𝙒/𝘾𝙃𝙍𝙄𝙎𝙏𝙈𝘼𝙎 𝙀𝘿𝙄𝙏𝙄𝙊𝙉 👻🩸</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h16phi</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1h16jdp</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the lines were a little difficult at the edges but I think they are perfect for me </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h16jdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1h16bgz</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t xml:space="preserve">created by Dayana Rodríguez </t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmfmlbojlg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1h15tt7</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was skeptical now liking </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhov21tkhg3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1h101a4</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I Saw the TV Glow Nails</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koa0ix2cre3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1h0zmbm</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My first Christmas set</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4ie3nxlle3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov 29 08:11:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_01.xlsx
+++ b/data/collected_data/2024_12_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C878"/>
+  <dimension ref="A1:C1059"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15361,6 +15361,3083 @@
         </is>
       </c>
     </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1h2h19x</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this! </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2h19x/love_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1h2gwt0</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Fall vibes</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00qt2igzrs3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1h2f4ct</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Practice makes progress 🥲</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrsa43666s3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1h2fap5</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Nightmare Pedicure</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2fap5/nightmare_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1h2g6lk</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>3-week old press-ons</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoteo0hkis3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1h2g5ye</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Wonderland  Nails </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2g5ye/winter_wonderland_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1h2fqg9</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Came out really shiny!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxhljmg5ds3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1h2feku</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Last fall nails of the year</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b1hd2bc9s3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1h2d1ps</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Hoping to get some ELI5 level answers to my questions about gel nails</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2d1ps/hoping_to_get_some_eli5_level_answers_to_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1h2efgp</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2efgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1h2dzxx</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Nail shape suggestions needed!</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giiq8kextr3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1h2dmfn</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Nails I did on my cousin</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2dmfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1h2di3o</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>November nail dump (I’m a nail tech and I specialize in hard gel manicures on natural nails)</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2di3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1h2c5ka</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Gel nail polish recommendation needed!!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2c5ka/gel_nail_polish_recommendation_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1h2b8x4</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to do with my nails </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2b8x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1h2c0mc</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Advice for a first timer</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2c0mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1h2blkv</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Subtle Christmas set</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2blkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1h2bfan</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>❄️ Winter Set ❄️</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7u47521c2r3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1h2bc4a</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Autumn</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfsxliee1r3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1h2b3qz</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>got my nails done for the very first time - I love it 😭❤️</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2b3qz</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1h2b1h2</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Possible DIY solution to gel lifting? </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2b1h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1h2az3t</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Framed insect nail art</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2az3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1h2a22g</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>3D nails</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0u1ruw4oq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1h29ofl</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Rate my apex!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h29ofl</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1h29e0p</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Gel x nail tips for tiny nail beds?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h29e0p/gel_x_nail_tips_for_tiny_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1h293tz</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>The cutest and most coquette nails you'll ever see in your life.</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2uecw3heq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1h28yer</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When your nail tech just gets you. </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gd85g8zcq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1h28urx</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it looks like the kirby's are floating </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h28urx</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1h28fyg</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>✨space shorties✨</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h28fyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1h28eey</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Starry night ⭐✨</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h28eey</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1h27nle</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Advice on durable fake nails for someone who has a hands on job</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it50u35e0q3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1h2808n</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Starry Night!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci1j0xgq3q3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1h27zet</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Cant stop looking at these🥹</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h27zet</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1h27vsp</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subtle and elegant design. </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u6cxd8k2q3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1h27pzp</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Magnet gel is my new current obsession</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2t8lb311q3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1h2720f</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with these metallic nails!!! </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cmw7kpwrup3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1h26z1q</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long nails for thanksgiving </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5192dcn4up3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1h26ees</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>First Set in Forever!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h26ees</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1h25qcq</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h25qcq/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1h264ar</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>🍁🍂Fall set🍂🍁</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4tz7i3ijmp3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1h25uub</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Winter nails for my mom ❄️</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h25uub</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1h25ubv</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Winter nails for my mom ❄️</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h25ubv</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1h25tyz</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Just finished this matte red set ♥️</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h25tyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1h22lam</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Environmental nail care</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h22lam/environmental_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1h1whn0</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I made these designs myself! Which one do you like best? I started in this world a short time ago. 🤭</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1whn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1h257t8</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Winter/Christmas nails</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h257t8</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1h25er0</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Finished Arcane and had feelings</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h25er0</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1h25bdp</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>My Tech literally waited for me to come in</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8koo3rhfp3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1h255kr</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been staring at these for almost 2 weeks and still can’t decide if they’re giving fall marble or poo smear… </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h255kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1h24434</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>I’m so in love with these! It’s giving icy snow queen ❄️💅</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h24434</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1h232xg</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Oh dear god</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eek1zqmhwo3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1h231q2</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>these are my natural nails. i’ve been told they look really pretty. are they? (also had to cut my pointer and thumb nails shorter)</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y98luf1wo3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1h22uvr</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with Essie Ethereal Escape plus Burgundy Bar by Gel Squad </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h22uvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1h22mk2</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech did her best </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h22mk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1h21wp1</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🥶🥶 </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h21wp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1h20fi0</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive and June </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h20fi0/olive_and_june/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1h1u64d</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel polish peeling off? </t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1u64d</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1h1t42u</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>First time getting nails done</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1t42u/first_time_getting_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1h21f9z</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Thanksgiving pie nails 🍁💅🏼🥧😊</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz2sc1n4jo3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1h203qy</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>💙 Blue Christmas Nails 💙</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl99jaes8o3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1h1zu2l</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Builder Gel Question</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1zu2l/builder_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1h1zsjg</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 1st set of Christmas nails this season. Thoughts? </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02qj1xpb6o3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1h1zfd9</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need help with stickers </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1zfd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1h1zcke</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Lucky 13 Lacquer - Throwin' Nightshade</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1zcke</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1h1y40w</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>You’re the Sunflower</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1y40w</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1h1wtkn</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Nails sore after manicure?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1wtkn/nails_sore_after_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1h1yte7</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Berry Fall Skittle 🍂🥀</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obzrk20iyn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1h1yn2c</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>My first chrome frenchies! This is who I am now</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1yn2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1h1yedt</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Y2k nails 😌♥️</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1yedt</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1h1yanv</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Polygel on top of tips</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1yanv</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1h1xr6t</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>new manicure</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0ukz18mpn3e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1h1xncc</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>some of my past sets 😁</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1xncc</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1h1wlkw</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Tried some character art for the first time; they've aged but they look happy 😊</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1wlkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1h1wazo</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really love my Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1wazo</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1h1wafq</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Am I the only one absolutely in love with this Color?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc9jm4crcn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1h1w5sr</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>French Jinx 💗💙</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sikvhjalbn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1h1vsa9</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Tropical pink and green set💚💗</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y79ydrx7n3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1h1vpu9</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Last fall set of the season 🍂🧡</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1vpu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1h1vf7l</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Sparkling neutral on natural nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2n1h10f4n3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1h1uzrn</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65th1fuyzm3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1h1uzgf</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there hope to strengthen my nails? </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlkuduavzm3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1h1uevq</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>3rd time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggmssohltm3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1h1ubk0</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Tis the season ❄️. Loved them so much 😍</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdgc1j3fsm3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1h1tuqn</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help to choose UV/LED lamp. </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1tuqn/need_help_to_choose_uvled_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1h1sxcl</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>getting into the christmas spirit</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zo6c0w5bm3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1h1ry9y</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Top 15 Pink Christmas Nail Trends to Try in 2024 &amp; 2025 💝</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h1ry9y/top_15_pink_christmas_nail_trends_to_try_in_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1h2gwf5</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Third mani this week</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fag0m14vrs3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1h2gtkr</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Emily de Molly - All the Rage</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2gtkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1h2gtb1</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>✨ Late B-day GITD lacquer showoff ✨</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2gtb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1h2f64v</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Bring your own polish?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2f64v/bring_your_own_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1h2eyf9</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Thanksgiving/first PPU mani</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2eyf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1h2evpj</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>I’m a failure!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2evpj/im_a_failure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1h2enqg</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">canadian rant </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2enqg/canadian_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1h2eezc</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Sassy sauce is BF sale is active now</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2eezc/sassy_sauce_is_bf_sale_is_active_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1h2eeyf</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Favorite scattered holo topper? Delicate</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2eeyf/favorite_scattered_holo_topper_delicate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1h2ecol</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked out at 8:59 sharp 😅 </t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wq95f9nxr3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1h2dnvy</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Dupes for Ethereal Lacquer’s Starborn?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2dnvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1h2dlf5</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>I'm a little late to the party...</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2dlf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1h2djey</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wearing a forgotten polish from my stash </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2djey</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1h2d31s</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>My preciouses</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2d31s</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1h2cxjj</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Lacquer 22 Black Friday sale</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2cxjj/lacquer_22_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1h2cndm</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>What do I do now?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2cndm/what_do_i_do_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1h2buzw</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Dupe for Starrily Northern Lights Simulator?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cg37wngv6r3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1h2bm00</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Best natural pink shimmer nail polish?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2bm00/best_natural_pink_shimmer_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1h2bg41</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Urban Outfitters has some Death Valley Nails shades on sale at 40% off!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx267dpk2r3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1h2ay4t</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Thanksgiving Mani! 🦃</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2ay4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1h2axkh</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Late Fall Skittle </t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2axkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1h2ap6e</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>On the hunt for a dupe of Orly: Elysian Field’s, or the real thing if someone knows where to find it! It’s the pretty-ugly I never knew I needed!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2ap6e/on_the_hunt_for_a_dupe_of_orly_elysian_fields_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1h2aat7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ilnp black friday started </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2aat7/ilnp_black_friday_started/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1h2a4my</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Fun with Flags</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2a4my</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1h2a1fm</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Hate that this smudged but here’s my Thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heatbhqynq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1h29yba</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>I’m new, excuse the ignorance..</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2m64kq3nq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1h28six</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basically my annual thanksgiving color </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aet11p2abq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1h28scu</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>first try at magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74yfldx9bq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1h27yeh</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Looking like lazer beams on my fingertips😍</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h27yeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1h27rhd</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can't decide if I love or hate this colour 🤣, thoughts? </t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcwn3g3d1q3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1h27n32</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>What I wore for thanksgiving</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h27n32</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1h27c45</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Thanksgiving skittle</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bitdk8gxp3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1h276h3</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Blue Lava by Cuticula</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h276h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1h27211</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Perfect nude shimmer ✨✨</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r18heogvup3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1h26rpo</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Paradox Polish Sit &amp; Spin PPU’ November 🧡💚</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h26rpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1h26j3z</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>My thermal obsession is only increasing as temps get colder 😍 Good Knight Polish - Just Here for the Lute</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h26j3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1h1z0q3</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Preschooler approved Thanksgiving skittle</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1z0q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1h25ji1</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Thanksgiving </t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6innjdhhp3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1h25dfv</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Are mooncat bottles still breaking?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h25dfv/are_mooncat_bottles_still_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1h2586r</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Opinions wanted: best black holo</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2586r/opinions_wanted_best_black_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1h24zun</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Fake Halo- nude with a twist!</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8dh1xnocp3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1h246ik</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Help me choose: Dream within a dream or Dam Polish Quantum Quest?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h246ik/help_me_choose_dream_within_a_dream_or_dam_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1h2453q</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">been feeling kinda blueeee </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2453q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1h23ch0</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>White spots on  nails, yesterday I've done press on nails with gel on top and took them off. i had no itching or redness and now this happened to my finger nails, also I've applied gel polish hours to see if I'm allergic to it but i had NO redness dryness, itchiness or swelling or thickness of nails</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h23ch0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1h2305d</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Show me your Thanksgiving manis! </t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgczke1vvo3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1h22tx2</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with Essie Ethereal Escape plus Burgundy Bar by Gel Squad </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h22tx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1h22lel</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thankful for "autumnal pink" </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h22lel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1h225wu</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wearing all brown for Thanksgiving so I wanted my nails to pop. Didn't realize I'd be so obsessed, I can't stop staring! </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h225wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1h220rc</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun quick mani I did today </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04zppwfwno3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1h21e4d</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Palette cleanser ✨️</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h21e4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1h216vj</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Just wanted to share one of my fave lacquers 😊</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h216vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1h2161t</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Subterfuge ✨</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2161t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1h20ir6</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Holo Taco-All birthstone polishes are coming back!!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/195wozb4co3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1h20e01</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best blurring base coats to hide nail line? </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h20e01/best_blurring_base_coats_to_hide_nail_line/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1h20c16</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Mooncat Fan</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h20c16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1h201x0</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>It breaks my heart when a pretty polish gets discontinued. 🥲</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h201x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1h20105</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I absolutely love HT Birthday Brat 💕 </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8btg8uv68o3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1h1zumh</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Happy Thanksgiving Y'all</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jeibpg5r6o3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1h1znje</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Looking for nice sheer sparkly nail polish for ugly hands owner 😭</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1znje/looking_for_nice_sheer_sparkly_nail_polish_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1h1zlv9</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My Thanksgiving nails!</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1zlv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1h1zju4</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Thanksgiving manicure</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rcj36rf4o3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1h1zdhn</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lucky 13 Lacquer - Throwin' Nightshade </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1zdhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1h1z18r</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Bonfire Dance, by Abomination Cosmetics 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1z18r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1h1ytfb</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llbt6ceiyn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1h1ypqp</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Berry Fall Skittle 🍂🥀</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2ymkuwnxn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1h1yfju</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>I never thought I’d love a yellow polish this much 🥹</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1yfju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1h1lko5</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>LF dnd dupe</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y22mt3tyj3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1h1y3sp</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - Merkitten </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1y3sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1h1xwlj</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>🦃 Thanksgiving mani</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nufsqpezqn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1h1xj06</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I just wanted to brag about my thumb</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1xj06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1h1x08r</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>First post and first skittle! Learning the basics ❤️</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxlbrs67jn3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1h1wua5</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>This weekends manicure pick</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1wua5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1h1wojh</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>heroes of lake huron: devin</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1wojh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1h1vvfc</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orly Replacement Brushes? </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h1vvfc/orly_replacement_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1h1veal</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Mooncat Midsummer's Dream gel?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhyvozg54n3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1h1uisj</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Dupe for Parasol by Blush lacquers?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1uisj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1h1txxq</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>My collection in Excel charts! Anyone else do something similar?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qrlldctnm3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1h1tt97</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>1 week checkin (Mooncat)</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1tt97</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1h1teq1</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>First GITD toy</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1teq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1h1srqt</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>For my fellow non-US lacqueristas…</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1srqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1h1s76t</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My blue and white french manicure </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1s76t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1h2aqrr</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like this design </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtsy96p9vq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1h2a7ky</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crackle nails make my shorties look good! I have a chrome (interference powder) addiction. </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ule1o8onpq3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1h27bp7</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Nail inspo</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h27bp7/nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1h27a2y</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Hand painted japanese text &amp; orchids duck nails</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h27a2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1h25xfh</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Karla Adame G.</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8ajud7ukp3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1h21tpn</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful creation by Dayana Rodríguez </t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iokhmzobmo3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1h21evu</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Thanksgiving pie nails 💅🏼🍁🥧</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvay0sd1jo3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1h20455</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>💙 Blue Christmas Nails 💙</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29ko6ocv8o3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1h1yy1g</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Hand-painted Doja Cat 'DEMONS' Nail Art from a while back</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1yy1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1h1we60</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>colorful I love it, always use the design that you like!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1we60</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1h1v25k</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Do You like this design?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpsid2zn0n3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1h1uxns</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Different kind of Christmas nail art </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sirqc14czm3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1h1tpbh</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Beach inspired press ons🏖🐠🦞</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h1tpbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1h1savb</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone snagged the Beetles Christmas Calendar yet?  It’s absolutely gorgeous! 😍 Can’t wait to grab one when it restocks! </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5frmc992m3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov 30 08:09:56 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_01.xlsx
+++ b/data/collected_data/2024_12_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1059"/>
+  <dimension ref="A1:C1224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18438,6 +18438,2811 @@
         </is>
       </c>
     </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1h36h68</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>I need some help with nail prep</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h36h68/i_need_some_help_with_nail_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1h367b3</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Something pink 🩷</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h367b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1h3608g</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">XXL Christmas Set❄️ </t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3608g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1h35d2l</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Took me 5 hours</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h35d2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1h34y0j</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t xml:space="preserve">after getting sns/acrylic nails since I was 13 im back to press ons </t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h34y0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1h34klw</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>I tried my best with my short nails</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h34klw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1h34gyq</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Press on Nails </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrg4s46fuy3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1h34byf</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Male manicure - if I had to paint one nail on each hand, which looks best?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h34byf/male_manicure_if_i_had_to_paint_one_nail_on_each/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1h33ury</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>First Time with Acrylics in over 2+ Years</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64a3o094oy3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1h33l73</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted simple fingers, but went crazy on toes. </t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h33l73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1h335m3</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>I have always wanted to try French nails but haven't been able to after consulting about my nails.What advice do you have foe me?</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h335m3/i_have_always_wanted_to_try_french_nails_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1h333ps</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I've always wanted to try French nails but haven't been able to after consulting about my nails. What advice do you have for me?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h333ps/ive_always_wanted_to_try_french_nails_but_havent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1h31kdx</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>First Christmas set of the season! ♥️</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h31kdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1h30x5q</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Love holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh9qxqhevx3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1h30pqp</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>First set of Holiday Nails 🎀✨️</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81l649gktx3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1h304l3</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Holidays!! </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m75ver8ox3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1h304eq</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Holidays!! </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtipjge6ox3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1h2zof7</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Christmas ❤️⛄🎄</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2zof7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1h2z5s7</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>What do you think about this?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9ys1s5sfx3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1h2yldq</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Anyone else love a lunula/half moon nail art design? 😻</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2yldq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1h2x3rw</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uipauajdyw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1h2x3ot</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Icy blue 💙</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtsozhucyw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1h2x36a</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying acrylic overlay, ombré nails </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvz8bro8yw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1h2wpmj</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Got my nails done! I'm definitely in love with these shades of blue 😍</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2wpmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1h2w0md</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feedback Needed </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1xkhovfpw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1h2vyk4</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2vyk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1h2v7ue</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails! </t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2v7ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1h2tr6h</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">That time my ‘marble’ attempt looked like prosciutto </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2tr6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1h2q1lb</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2q1lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1h2tbe2</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Winter cute dear</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2tbe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1h2t5ti</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Vacation nails 🫶</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2t5ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1h2ssag</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>now that temps in NC are finally below 60 degrees… ❄️🤍🤣</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1afs8v4ozv3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1h2srmv</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>I’m loving this color for November</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61ami9sizv3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1h2slyg</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Base coat is SO IMPORTANT!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2slyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1h2s86l</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Do these look natural?</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2s86l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1h2s7c8</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Velvety Black Cherry Nails</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2s7c8/velvety_black_cherry_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1h2rrnm</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting better </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2rrnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1h2rlhw</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Halcyon 💜</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7tphb1kqv3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1h2qi4j</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let it Snow - Snowflake and glitter nails </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjp6bq52iv3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1h2q9vp</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>I’m an right arm amputee but still always keep my left hand cute and done 💋❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2q9vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1h2q6j4</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Chocolate w/ blue green glitter 🪩</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2q6j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1h2pb13</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Nail set for Apocalypse Fest this weekend 🖤🕷️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2pb13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1h2p8ui</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Hand painted mushrooms!!! BIAB</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2p8ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1h2p5y9</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Holiday nails and the first snow</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2p5y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1h2oeiq</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Bad press on job???</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2oeiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1h2nxch</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>🎄 Simple Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0piipa9dxu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1h2np49</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>🧸</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2np49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1h2nj3w</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Winter nails are my favourite, you can make simple manicures pop with a bit a glitter ✨</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2nj3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1h2nax4</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Ready for December (and also Wicked) ✨</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4z1o7w1su3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1h2cvf6</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Took me 4.5 hours</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2cvf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1h2grln</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is this nail product called? </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2grln/what_is_this_nail_product_called/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1h2ib4x</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>several nails splitting horizontally (on the pink part)</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2ib4x/several_nails_splitting_horizontally_on_the_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1h2n0sf</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Icy 🥶❄️</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hymlf6mpu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1h2mc1k</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Unsure if i like it..red might be too much.🤔</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c6559zoju3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1h2lnxb</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>It’s almost frosty season ❄️☃️</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7d58ttadu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1h2k7hv</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Catrice Lacquer - lighting doesn't do them justice!</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqkmr2k0yt3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1h2j5ql</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Seller Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2j5ql/seller_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1h2ius1</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Christmas Nails💅🏾🎄</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkpyk8a5ht3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1h2ioxk</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">White nails for a fresh, clean look! </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2ioxk/white_nails_for_a_fresh_clean_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1h2igld</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying to do gel x nails </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2igld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1h2i8zu</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Rubber base/Builder gel under PRESS-ONS to protect?!</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h2i8zu/rubber_basebuilder_gel_under_pressons_to_protect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1h2i5cf</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Doll Nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2i5cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1h2hipj</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>✨ Late B-day GITD polish of choice ✨</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2hipj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1h2hhhs</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>🤎✨</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2hhhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1h37twq</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Hey Australians</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h37twq/hey_australians/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1h37svs</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Brushes</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h37svs/brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1h377hb</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Holo Taco - Nightshade</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h377hb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1h374bb</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can someone please recommend a dupe for Polished for days 2024 nail polish? </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h374bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1h372at</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Hedgerow green</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h372at</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1h36c06</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Final polish purchase of 2024</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nybn4hsdez3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1h369zg</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I'm on DAY 32 of a mani I started on October 28th!!  1st time posting photos of my progression of coats and effects...  Full disclosure - I'm a newbie to effects like French and ombré</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>/r/Nailpolish/comments/1h319x8/im_on_day_32_of_a_mani_i_started_on_october_28th/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1h35zp0</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Dark nude that already has large silver glitters in it?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h35zp0/dark_nude_that_already_has_large_silver_glitters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1h35ta7</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>My Thanksgiving Mani, LynB - Aquarius (The Water Bearer)</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h35ta7/my_thanksgiving_mani_lynb_aquarius_the_water/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1h351v2</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>BKL Dupes for Queen Of Rot</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h351v2/bkl_dupes_for_queen_of_rot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1h34tye</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>My mooncat cart as a first time buyer</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h34tye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1h34qub</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Staining of sidewalls</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h34qub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1h34qbl</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>First time ILNP order</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h34qbl/first_time_ilnp_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1h34kib</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ghosts of a Hecate polish </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dcjzrmncvy3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1h34jcy</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Great Lakes lacquer still has a ton of polishes for sale!!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h34jcy/great_lakes_lacquer_still_has_a_ton_of_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1h34fj6</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>First black Friday haul. Which would you be most excited to try first out of this list?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h34fj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1h33w8b</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>ILNP Velvets</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md5n795joy3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1h33rgx</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Late Thanksgiving mani post!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3kw52p2ny3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1h33m8y</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>ILNP 30# magnet?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h33m8y/ilnp_30_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1h33jcw</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Different Dimensions?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h33jcw/different_dimensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1h33fm0</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Canadian Laqueristas, any issues with Black Friday Shipping?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmu1bjxsjy3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1h33c13</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>All of the faces of Fashion Polly</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h33c13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1h32rk9</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>The end of a 10-year dupe quest</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h32rk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1h32lvb</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Feeling Fizzy</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63kn4ou9by3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1h32bea</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h32bea/great_lakes_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1h31t9x</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Tips for very short and flat nails</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h31t9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1h31qnw</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>that’s it that’s all i’m done</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vk363jy43y3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1h31656</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Am I the only one that can’t buy Whatcha Indie on By Dany Vianna anymore?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h31656/am_i_the_only_one_that_cant_buy_whatcha_indie_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1h30knl</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>She betrayed me 😔</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i85s6sb9sx3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1h30i6l</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My final BF polish order </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1j7fs8mrx3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1h2zwkz</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Cirque mini snapped while opening - can I save it?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2zwkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1h2ze1u</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>First Christmas manicure! Ahhh!! 🎄</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5621a49shx3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1h2z5hk</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with my first glisten &amp;glow purchase </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2z5hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1h2yy9u</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I am out of control 😭</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2yy9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1h2ydpa</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One year difference </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrqtesq79x3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1h2xg66</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I’m getting better at this! </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2xg66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1h2wy18</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Drugstore Holiday</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2wy18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1h2wxe4</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Hi 👋🏻 Is Seche Vite supposed to be very thick? I think mine is getting too thick and not drying properly.</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2wxe4/hi_is_seche_vite_supposed_to_be_very_thick_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1h2wwda</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soo... Nailland is ripping people off with their policies </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2wwda/soo_nailland_is_ripping_people_off_with_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1h2w5uz</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Who is done BF shopping?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2w5uz/who_is_done_bf_shopping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1h2w0ig</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Calling all long stiletto/pointy nail ladies with natural nails</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2w0ig/calling_all_long_stilettopointy_nail_ladies_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1h2vzpa</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>So flashy 🤩</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7lt61a98pw3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1h2vriz</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Dupe for “handpicked for me” by sephora by opi</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2vriz/dupe_for_handpicked_for_me_by_sephora_by_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1h2vhfa</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Cranberry red</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7odeg4v2lw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1h2vb91</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Norpsilocin by Clionadh</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jliba07njw3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1h2v3b2</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Black Friday sale kbshimmer!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2v3b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1h2v2oi</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Psa: Clionadh restocked their psilo magnetic trio</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk9qkgdrhw3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1h2v1yf</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Tropical heatwave won't scratch the goblins and ghoulies itch.</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2v1yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1h2urrh</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Cirque Color</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2urrh/cirque_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1h2ulow</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This polish was the definition of 'trust the process' but it all paid off in the end! </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2ulow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1h2ul29</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI x Wicked Ozmopolitan </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6rvo13sdw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1h2u6rg</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>My nails accidentally matched my dog’s DNA test kit!</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqdcw7gkaw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1h2u1bk</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>First time using builder gel, I’m obsessed !!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2u1bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1h2tziu</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Tried to make my nails look like liquid glass</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2tziu/tried_to_make_my_nails_look_like_liquid_glass/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1h2tu2o</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fire + Flannel </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2tu2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1h2ts4c</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cupcake Polish- Blue Tourmaline </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vcuwm3a7w3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1h2ticp</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>November nails</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2ticp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1h2td3w</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Birthday nails ✨</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2td3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1h2rzay</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Can I paint over Gelx or should I go in?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0eh62tsgtv3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1h2rinf</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First holo taco manicure </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c55bxmvwpv3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1h2rhql</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Halcyon 💜</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyk3frrppv3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1h2r0tc</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Quick Dry Top Coat</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2r0tc/quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1h2qlm5</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco Moon Lagoon and Vitamin Glow </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2qlm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1h2q7lg</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Nail hardener that can be a base and top?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2q7lg/nail_hardener_that_can_be_a_base_and_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1h2q1k9</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite Subtle Shimmers? </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co2fr7cjev3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1h2pjae</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Y'all, I need to find me more polishes that look similar to this one and would really love suggestions!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34z5yeo29v3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1h2pci0</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>💎💚Emeralds💚💎</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2pci0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1h2p5wy</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Who knew you could do your nails in an hour? (It was all of you and you were right!)</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zq7lwtj7v3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1h2owe7</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Add length temporarily without damaging natural nail?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2owe7/add_length_temporarily_without_damaging_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1h2otuz</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Perfect thanksgiving color</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2ob70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1h2e6y2</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>SOS: is there hope after gel allergy?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2e6y2/sos_is_there_hope_after_gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1h2nvyf</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for a polish from mid 2010s</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2nvyf/looking_for_a_dupe_for_a_polish_from_mid_2010s/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1h2nrd2</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Time for a classic</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef23t82yvu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1h2nk0e</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>I feel this is close to a good nude for me. (Essie the struggle is real)</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2nk0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1h2mzk8</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>I’m a convert to velvet nails!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1halcatapu3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1h2moiu</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Inventory before shopping Zoya’s Black Friday sale</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jguxadhtmu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1h2l641</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>kbshimmers base coats?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2l641/kbshimmers_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1h2kgly</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aar7xaaw0u3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1h2k40n</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Caprice Gel Lacquer 163</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pt2blquwt3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1h2jngs</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any affordable/good UV gel polish brands that deliver to Austria/EU? </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h2jngs/any_affordablegood_uv_gel_polish_brands_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1h2hhp7</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>✨ Late B-day GITD polishof choice ✨</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2hhp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1h37qkr</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nail Art ideas </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h37qkr/christmas_nail_art_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1h36585</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Christmas Set❄️💙 Polygel Edition✨</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/powxk3cacz3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1h35k29</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Fancy French Nails UV Gel</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h35k29</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1h34tpu</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>MUST-TRY beginner technique</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuxzt264yy3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1h34hqe</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Press on Nails </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5yd5jrmuy3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1h31jxk</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Homemade nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h31jxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1h2yeoz</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to keep silver beads from getting scratched? :(( </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h2yeoz/how_to_keep_silver_beads_from_getting_scratched/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1h2wa0z</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Winter Wonderland ❄️</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2wa0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1h2vkj9</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>thi blue is perfect for a graduation, is one of my fav ones</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah30d5lmlw3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1h2v9j0</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2v9j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1h2t9zv</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Winter cute dear</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2t9zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1h2qybx</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>galaxy theme! by margg.nails</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsyoryohlv3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1h2pmf0</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Holiday Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2pmf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1h2omyv</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">deep blue and light blue with some powder i loved it </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2omyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1h2nx33</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>🎄 Simple Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v1kvt6bxu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1h2n1aa</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Christmas candles</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ht4z64qpu3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1h2mtsm</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand-sculpted Clicker/The Last of Us Nail Art </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h2mtsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1h2mrii</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love the purple of my nails </t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwt6r6iknu3e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1h2kzwn</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Karla Adame G </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3p4g9ak6u3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1h2jwsf</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You’re a mean one, Mr Grinch </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay2nj29gut3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec  1 08:09:59 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_01.xlsx
+++ b/data/collected_data/2024_12_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1224"/>
+  <dimension ref="A1:C1425"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21243,6 +21243,3423 @@
         </is>
       </c>
     </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1h3y9uy</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg2u27bdz64e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1h3y8kp</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3y8kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1h3y0fb</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Where do I start?</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3y0fb/where_do_i_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1h3xy0m</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>New set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gsbt9s4v64e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1h3xwlv</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter nails ❄️ ⛄️ </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3xwlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1h3xkyf</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>trial christmas nails 🎁</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0adlkfoq64e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1h3xnfn</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nail lady eat ?? </t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3xnfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1h3x6oq</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>winter fill! 🩵</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3x6oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1h3vf40</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Ways to get your nails to grow long and healthy? (Two-part question-Sorry)</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3vf40/ways_to_get_your_nails_to_grow_long_and_healthy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1h3vvb6</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>So.. can you use a nail primer with press ons?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3vvb6/so_can_you_use_a_nail_primer_with_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1h3wpj6</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i had these done a while ago but decided to share them here!! 💗✨ </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5pwawedg64e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1h3vwuq</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling festive </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3vwuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1h3vt4s</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Always struggle with press-ons</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3vt4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1h3vo52</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>First time doing my own gels</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3vo52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1h3v7g1</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>one last fall set</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hulwhwjl064e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1h3uyie</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Press on nails for water park and swimming?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3uyie/press_on_nails_for_water_park_and_swimming/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1h3sp4t</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Sculpture/builder/liquid different?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3sp4t/sculpturebuilderliquid_different/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1h3urpf</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Christmas set I did yesterday </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ppofv62w54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1h3ura1</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>December nails 💅🏻🎀</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ciokvuuxv54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1h3ue7p</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Very happy with my natural nail length ❤️</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3ue7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1h3uamb</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Grinchmas Set 💚</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3uamb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1h3tyak</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>What can I do until my nail grows back out?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3tyak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1h3txw7</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Near christmas! </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3txw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1h3trsy</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>I need ideas</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2z9q8x7m54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1h3tqae</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>loveeee</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e664nq5tl54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1h3tmqa</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3tmqa/oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1h3tl1l</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Santa nails!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwhytr7fk54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1h3tbci</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>[Ferro]Magnetic Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80krv13wh54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1h3sxat</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue on my natural nails </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3sxat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1h3slh8</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>first attempt at flowers!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gesju6wa54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1h3sdxu</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter ❄️ </t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h09e8xy854e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1h3sdu6</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snowflake </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6compr7y854e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1h3s8qy</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Press ons 🌿</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4ybi4pl754e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1h3rzif</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Learning gel x</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buzdsz48554e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1h3rivp</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Was supposed to be deer nails but I messed up the fur painting lol</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3rivp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1h3r2cj</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>It’s tiiiimmmeeeee ❄️ 🎄</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vt4tqt9sw44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1h3r19g</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tis the season! </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gmo1qbiw44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1h3qxee</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Peppermint nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe6sihckv44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1h3qx5z</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>new set 🐆🎀</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3qx5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1h3qsga</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Trouble knowing what nail shape would match my fingers?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3qsga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1h3qrix</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cutest mani </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3qrix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1h3qfjg</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Just why</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hyxfqf7r44e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1h3qcvf</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">green french tips for winter </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikz83g2lq44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1h3qc5h</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I’m obsessed with my nails.</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16cnl4qeq44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1h3q8xn</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Went a bit longer with my new set 😍</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybdvne0np44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1h3q13a</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>is there a way to change the base color on press ons?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snvybu5wn44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1h3o16t</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Light Elegance Hard Gel </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3o16t/light_elegance_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1h3pukh</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>My nails look so much nicer now with my new engagement ring 🥰</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znglp4ibm44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1h3pq18</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>French nails</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3pq18/french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1h3poa8</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Claw nails c:</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3poa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1h3pgb7</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>First set from a new place</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzxsjmhvi44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1h3pf2u</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polar Vortex 🥶❄️ (fitting now that it’s 20° in SC) </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3pf2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1h3pedm</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>GelX - Coffin - Cat Eye - Jelly - Chrome</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcu6779fi44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1h3oyjg</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with my vacay nails </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pyyqsske44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1h3owym</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>ready for the holidays 😋❄️</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5x1oie7e44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1h3oguy</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Milky white might be my new favourite </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54ws3naga44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1h3nuta</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Waar kopen jullie je favoriete nagellijm?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3nuta/waar_kopen_jullie_je_favoriete_nagellijm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1h3nula</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>I think I'm getting engaged on Monday, I need nail ideas!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3nula</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1h3ntgs</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails on my mum </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mthnng1544e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1h3n4vx</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>How do you find the dream nail tech/salon?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3n4vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1h3ngwl</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>How do we feel about these holiday nails?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3ngwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1h3n2g7</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>finally tried OPI “bubble bath” and i totally get the hype now</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3n2g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1h3mgzn</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Kinda Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3mgzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1h3mdg2</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>DIY Christmas Set 🎄</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3mdg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1h3mctr</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Long overdue 💙</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3mctr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1h3m3ss</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5qww91sq34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1h3m59j</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>DIY Nails</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmcbibz4r34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1h3lszc</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Burgundy 🍒🔴</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3lszc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1h3lo9w</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>This red with glitter is FIREEEE</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgh51n49n34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1h3llc5</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Had this mani for Thanksgiving</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3llc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1h3iywu</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Is there any way to make my nails stop growing as fast?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3iywu/is_there_any_way_to_make_my_nails_stop_growing_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1h3grth</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Best European gel starters kit?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3grth/best_european_gel_starters_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1h3ky0o</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I find it very brat to have brat nails during winter💚</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3ky0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1h3klrr</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>I really should start painting them b4 I put them on</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3klrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1h3khlv</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄⛄️</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3khlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1h3k5no</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Ready for Christmas.</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3k5no</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1h3jvw7</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I kinda hate them? </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3jvw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1h3jmpj</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>i'm finally winter ready! ❄️</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3jmpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1h3jk29</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>French mani. 🤍🩷</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgyxa6u2634e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1h3idgf</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Should I change the red nail to green?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9bwaawgw24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1h3i9rd</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech is the best </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8q0a2aov24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1h3i39s</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Hello, what do you think for my first job?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpnwp6p6u24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1h3hvth</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Is this a fall or winter color?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejkx7gdis24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1h3hlzx</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Advice requested</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3hlzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1h3hgrp</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>New DIY polygel set, not sure about the shape</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3hgrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1h3hep4</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Alexa play Snowman ☃️❄️🎄</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3hep4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1h3he7r</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s time! </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awfzq2slo24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1h3h6sy</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time getting a shape other than coffin! </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3em628mzm24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1h3h3z6</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>A long shot but looking to find this shellac polish. I love it so much, but almost no nail salons carry this line! It’s soo sparkly 💜</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sz3toy4dm24e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1h3gz9u</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Loving this color 🥰</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b34ri2lcl24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1h3ge9q</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>My nails have never been this long!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nw5lymmvg24e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1h3g3ol</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Beetles Advent Calendar Canada</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3g3ol/beetles_advent_calendar_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1h3fuzj</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Press ons Question! Anyone know why my glitter ones stay on longer?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3fuzj/press_ons_question_anyone_know_why_my_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1h3fthb</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Obsessed 🎀</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2icd9etac24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1h3fsvk</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>A question about nail strengtheners...</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h3fsvk/a_question_about_nail_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1h3dq4p</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>why??</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pczziv8du14e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1h3drat</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please give me feedback </t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3drat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1h36d6x</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>I'm on DAY 32 of a mani I started on October 28th!! 1st time posting photos of my progression of coats and effects... Full disclosure - I'm a newbie to effects like French and ombré</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h36d6x/im_on_day_32_of_a_mani_i_started_on_october_28th/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1h353mz</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Any good ways to keep a broken nail together permanently?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h353mz/any_good_ways_to_keep_a_broken_nail_together/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1h31jtl</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Too boring or tacky?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsfw04ta1y3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1h3xiz9</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Unintentional twins fr 🍒</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/daorync0q64e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1h3xeui</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>KBShimmer Gel Cuticle Remover and tool recs?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3xeui/kbshimmer_gel_cuticle_remover_and_tool_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1h3w1bf</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>My first big haul for Black Friday as a Christmas present from my mom and fiancé!</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3w1bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1h3vlwk</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Mooncat Question</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejz0tzaq464e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1h3v667</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found discontinued topcoat Revlon </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3v667/found_discontinued_topcoat_revlon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1h3uscb</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>feelin like a fairy 🧚‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vfjmub52w54e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1h3ulwx</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Light blue skittle</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3ulwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1h3u3o2</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> November Polished</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3u3o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1h3u1vo</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Mooncat Artemis’ Deathkiss</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3u1vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1h3tvzu</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Multichrome pigment question </t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3tvzu/multichrome_pigment_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1h3tjtk</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Nail Junkie</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/22-11-2024-NpXtUIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1h3thtm</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do Zoya polishes wear longer than others? </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3thtm/do_zoya_polishes_wear_longer_than_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1h3t1x5</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>What I wore in November</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3t1x5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1h3suvf</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Wicked Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcw5ctecd54e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1h3srum</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Poseidon's Prize</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1wgrk0kjc54e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1h3s49k</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regular polish French tip node </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiu27oxf654e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1h3rvo1</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Poems for a Harvest Moon</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3rvo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1h3rgs1</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>ILNP Deep space</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3rgs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1h3r6j8</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>This glowy shift is unreal!</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wzfwq8px44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1h3q3j3</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>more intense shimmer dupe for essie "you do blue"</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3q3j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1h3pvb5</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark Horse at Dutch Bros </t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3pvb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1h3pufu</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Similar frosted metals to Holo Taco’s? </t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz1z5mlam44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1h3pswf</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Can’t stop staring</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dwjodmwl44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1h3pgud</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Dark Winter Skittle</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dya7yxq0j44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1h3pddi</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Jewel Beetle is stunning 🪲</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3pddi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1h3pd47</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polar Vortex 🥶❄️ (fitting now that it’s 20° in SC) </t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3pd47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1h3pa6d</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tell me about your storage systems </t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3pa6d/tell_me_about_your_storage_systems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1h3p9zz</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Your Favorite 'Beetle-esque' Polish?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n422nbvch44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1h3owbd</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>So this is love.</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bdzphf1e44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1h3opuo</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>It finally happened...</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oe23flkc44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1h3oosy</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Hello Holiday’s!</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3oosy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1h3okiz</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>First Thermal ! 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3okiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1h3ohif</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What top coat do you use and how long does it take on average for your polish to fully dry? Also, is there a fool proof way you’ve found to test the “dryness” of your polish without ruining your manicure? </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3ohif/what_top_coat_do_you_use_and_how_long_does_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1h3ob68</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Pale lavender on this crisp fall day</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbgci2i4944e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1h3nwih</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>What’s the deal with Starrily?</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3nwih/whats_the_deal_with_starrily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1h3nsp3</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Turns out the only thing I wanted from Mooncat isn't included in their "Sitewide" sale. </t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3nsp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1h3nnkx</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>How do I know if any of these are vintage?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdryrcvn344e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1h3njj1</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>My Thanksgiving Mani</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3njj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1h3ni87</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Nail damage</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3ni87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1h3myjs</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Best Lighting/Lamp?</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3myjs/best_lightinglamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1h3mubw</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a dark green jelly </t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flrke9fww34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1h3moud</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Double Glitter  Crackle</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3moud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1h3mjge</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupes for this colour? Can’t find anywhere </t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3mjge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1h3ltpp</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Terrazzo topcoat?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3ltpp/terrazzo_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1h3lpr2</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Slots of fun Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3lpr2/slots_of_fun_sassy_sauce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1h3loyn</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Newb November - Matched my nails to my outfit for once 🍏🍏🍏</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3loyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1h3liqu</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>No one else in my life will understand what a responsible use of my BF budget this was 😂🫣</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3liqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1h3linp</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>My last fall mani of the year</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xzo5hsyl34e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1h3l9ca</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Does this exist?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3l9ca/does_this_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1h3l8rk</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer Opinions?</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb78ghxqj34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1h3l6qt</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Wintery polish time!</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amnee03aj34e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1h3kyj6</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>I think that Psilocybin is my new favorite magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gxyn1hveh34e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1h3kx3t</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>LynB Designs rewards question</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3kx3t/lynb_designs_rewards_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1h3knmc</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Does anyone know of a dupe for Ethereal Lacquer Flutter?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txc8b3fxe34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1h3k4mc</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce appreciation </t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3k4mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1h3jq9d</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Winter Vibes ❄️☃️🥶</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhrb5omf734e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1h3jigl</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feel like a unicorn 🦄 </t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3jigl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1h3j795</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Really happy at the current length of my nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhlt2dp8334e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1h323py</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>How to take better nail pictures</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h323py</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1h32pfz</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>New to Nails, Here is my first haul!!</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h32pfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1h35ndg</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Hunting for Purple Nail Polish with Orange Sheen</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h35ndg/hunting_for_purple_nail_polish_with_orange_sheen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1h36kpg</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Has USPS insurance ever paid for  nail polish they lost or destroyed?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h36kpg/has_usps_insurance_ever_paid_for_nail_polish_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1h3fcbr</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Jewel Beetle vs KBS For the Pun Of It </t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3fcbr/mooncat_jewel_beetle_vs_kbs_for_the_pun_of_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1h3iqhl</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>First attempt at marble nails, how did I do?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3iqhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1h3iucz</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>November Mani Round Up</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3iucz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1h3irup</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Anyone have a dupe?</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr9mvw4rz24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1h3hrt8</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Anyone have experience with stickers?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gkldzlir24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1h3h6lq</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Pop-arazzi transition to Miss Spa, color differences</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3h6lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1h3h49d</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just need to gush about Urban Wasteland from Prisim Parade </t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3h49d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1h3h17l</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Not gonna lie....the shipping hurts a bit😭😭</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwogj5yll24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1h3ggen</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>What’s everyone’s favorite low effort but looks expensive polish or combo</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m9z8q4dh24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1h3fk93</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Searching for Pure Ice Tame Me Now dupe</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://megis217.wordpress.com/2013/02/26/pure-ice-nail-polishes-of-2013-swatchfest-part-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1h3fhhz</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Absolute Mess that was the Great Lakes Lacquer BF 2024 Event </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4khvnppm924e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1h3f09x</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>do you remember your first? 💅</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3f09x/do_you_remember_your_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1h3etbt</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Is it possible to add more to an order at Nailland.hu?</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>/r/EUnails/comments/1h3eslq/is_it_possible_to_add_more_to_an_order_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1h3engk</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Question about swatching</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3engk/question_about_swatching/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1h3eaw6</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Teal to purple to pink.</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3eaw6/teal_to_purple_to_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1h3e5ca</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Shorty manis of November</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3e5ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1h3e58h</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Emily de Molly Oceanic &amp; Eternal Forces</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3e58h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1h3dycr</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>DIY Advent Calendar</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3dycr/diy_advent_calendar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1h3dxeo</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>How good is dirtbag, death valley nails?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3dxeo/how_good_is_dirtbag_death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1h3d72y</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>I didn’t expect to love these polishes together so much!</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3d72y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1h3ctsh</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Can anyone tell me where can I find this pink?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbv24dgsl14e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1h3bnoj</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Breaking out of my comfort zone with OPI All Your Dreams in Vending Machines</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sl3bhyo914e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1h3bmvq</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Thermal AND magnetic polish</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3bmvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1h3afu5</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little bit in love </t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1ht05gyu04e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1h3a31t</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Uk based - where do you get your polish without spending more on shipping than the item itself?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h3a31t/uk_based_where_do_you_get_your_polish_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1h38dgc</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Am I crazy for getting all three of these???</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jhv7735304e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1h3qxri</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Peppermint nails ❄️💕💅🏼</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eou7iornv44e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1h3qr1y</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Green nail for the green dress</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3qr1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1h3myaa</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Almond roses 🩷</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf7iwjksx34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1h3ksjy</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>First gel X nails!</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5gi0213g34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1h3k72f</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Holiday Set!</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unqej4w7b34e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1h3iv2i</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Inspired by Sneakers</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3iv2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1h3ibcx</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lisa Frank inspired </t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq8y5o10w24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1h3hfoj</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Alexa play Snowman ☃️❄️🎄</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3hfoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1h3guw0</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>My first sets</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krbmqarik24e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1h3fgnk</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>☯️🤍🖤</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xboaq3ze924e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1h3e1r4</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>pet nails!</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h3e1r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1h3d1in</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Another simple christmas design 🤍</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5fi9h6yn14e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1h3c5or</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Meraki nail's</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eqsu503f14e1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>